<commit_message>
rebuilding site Thu 07 Oct 2021 01:08:12 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/bendingData.xlsx
+++ b/engineering/courses/mae101/docs/bendingData.xlsx
@@ -232,7 +232,6 @@
       <t xml:space="preserve">Width (w) = 1.509 in
 Length (L) = 35.875 in
 Thickness (t) = 0.255 in
-	Inertia (I) = (w^3*t) ∕ 12    in^4
 	Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -385,7 +384,6 @@
       <t xml:space="preserve">Width (w) = 0.255 in
 Length (L) = 35.875 in
 Thickness (t) = 1.509 in
-Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)
 Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -407,7 +405,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> psi	</t>
+      <t xml:space="preserve"> psi</t>
     </r>
   </si>
   <si>
@@ -947,18 +945,171 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285840</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>259920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1504440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>811800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6597000" y="7864560"/>
+          <a:ext cx="1218600" cy="551880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>897840</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>451800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1926000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>898920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7209000" y="10622520"/>
+          <a:ext cx="1028160" cy="447120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>167760</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>182520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>375480</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1029600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1487880" y="7787160"/>
+          <a:ext cx="1599480" cy="847080"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266040</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>182520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>750960</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1244160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1586160" y="10353240"/>
+          <a:ext cx="484920" cy="1061640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.99"/>
@@ -1775,7 +1926,7 @@
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
     </row>
-    <row r="40" customFormat="false" ht="84.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="110.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="7" t="s">
         <v>26</v>
       </c>
@@ -2191,5 +2342,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rebuilding site Thu 07 Oct 2021 01:18:57 PM EDT
</commit_message>
<xml_diff>
--- a/engineering/courses/mae101/docs/bendingData.xlsx
+++ b/engineering/courses/mae101/docs/bendingData.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t xml:space="preserve">Bending Of Beam Raw Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inertia (I) = (w^3*t) ∕ 12    (lb∙in2)</t>
   </si>
   <si>
     <t xml:space="preserve">RAW Data 1</t>
@@ -48,7 +45,6 @@
       <t xml:space="preserve">Width (w) = 1.427 in
 Length (L) = 35.875 in
 Thickness (t) = 0.273 in
-	Inertia (I) = (w^3*t) ∕ 12   in^4
 	Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -85,7 +81,6 @@
       <t xml:space="preserve">Width (w) = 1.54 in
 Length (L) = 36 in
 Thickness (t) = 0.22 in
-	Inertia (I) = (w^3*t) ∕ 12    in^4
 	Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -111,22 +106,48 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">P load (lb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ho</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Inertia (I) in</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Experimental deflection ∆h (in)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Theory deflection ∆h (in)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Weight (lb)</t>
   </si>
   <si>
-    <t xml:space="preserve">H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ho</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inertia (I)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Experimental deflection ∆h (in)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Theory deflection ∆h (in)</t>
   </si>
   <si>
     <t xml:space="preserve">Case 2: Wood beam - thin side on support</t>
@@ -143,7 +164,6 @@
       <t xml:space="preserve">Width (w) = 0.273 in
 Length (L) = 35.875 in
 Thickness (t) = 1.427 in
-Inertia (I) = (w^3*t) ∕ 12    in^4
 Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -180,7 +200,6 @@
       <t xml:space="preserve">Width (w) = 0.22 in
 Length (L) = 36 in
 Thickness (t) = 1.54 in
-Inertia (I) = (w^3*t) ∕ 12    in^4
 Elasticity (E) = 2*10</t>
     </r>
     <r>
@@ -204,6 +223,12 @@
       </rPr>
       <t xml:space="preserve"> psi</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">H (in)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ho (in)</t>
   </si>
   <si>
     <t xml:space="preserve">Experimental ∆h (in)</t>
@@ -276,7 +301,9 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">= 31.25 inch, P= load, </t>
+      <t xml:space="preserve">= 31.25 inch, 
+P= load, 
+</t>
     </r>
     <r>
       <rPr>
@@ -297,7 +324,8 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = 1.007 inch, </t>
+      <t xml:space="preserve"> = 1.007 inch, 
+</t>
     </r>
     <r>
       <rPr>
@@ -318,7 +346,8 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">= 0.130 inch, </t>
+      <t xml:space="preserve">= 0.130 inch, 
+</t>
     </r>
     <r>
       <rPr>
@@ -364,13 +393,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Load(lbs.)</t>
+    <t xml:space="preserve">P  Load(lbs.)</t>
   </si>
   <si>
     <t xml:space="preserve">Experimental deflection (inch)</t>
   </si>
   <si>
-    <t xml:space="preserve">Aluminum beam (short side on Support)</t>
+    <t xml:space="preserve">Aluminum beam (thin side on Support)</t>
   </si>
   <si>
     <r>
@@ -428,7 +457,9 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">= 35 inch, P= load, </t>
+      <t xml:space="preserve">= 35 inch, 
+P= load, 
+</t>
     </r>
     <r>
       <rPr>
@@ -449,7 +480,8 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = 0.130 inch, </t>
+      <t xml:space="preserve"> = 0.130 inch, 
+</t>
     </r>
     <r>
       <rPr>
@@ -470,7 +502,8 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = 1.007 inch, </t>
+      <t xml:space="preserve"> = 1.007 inch, 
+</t>
     </r>
     <r>
       <rPr>
@@ -514,6 +547,9 @@
       </rPr>
       <t xml:space="preserve"> psi  </t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">P Load(lbs.)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +560,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -572,6 +608,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -817,6 +861,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -825,20 +885,88 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -847,90 +975,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -950,15 +994,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>285840</xdr:colOff>
+      <xdr:colOff>266040</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>259920</xdr:rowOff>
+      <xdr:rowOff>245520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1504440</xdr:colOff>
+      <xdr:colOff>1484640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>811800</xdr:rowOff>
+      <xdr:rowOff>797400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -971,7 +1015,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6597000" y="7864560"/>
+          <a:off x="6577200" y="8018280"/>
           <a:ext cx="1218600" cy="551880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -987,15 +1031,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>897840</xdr:colOff>
+      <xdr:colOff>365040</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>451800</xdr:rowOff>
+      <xdr:rowOff>293400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1926000</xdr:colOff>
+      <xdr:colOff>1393200</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>898920</xdr:rowOff>
+      <xdr:rowOff>740520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1008,7 +1052,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7209000" y="10622520"/>
+          <a:off x="6676200" y="10632240"/>
           <a:ext cx="1028160" cy="447120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1024,15 +1068,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>167760</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>182520</xdr:rowOff>
+      <xdr:colOff>207000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>375480</xdr:colOff>
+      <xdr:colOff>394920</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>1029600</xdr:rowOff>
+      <xdr:rowOff>1067400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1045,8 +1089,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1487880" y="7787160"/>
-          <a:ext cx="1599480" cy="847080"/>
+          <a:off x="1527120" y="7671960"/>
+          <a:ext cx="1579680" cy="1168200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1061,15 +1105,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>266040</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>182520</xdr:rowOff>
+      <xdr:colOff>88560</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>11520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>1244160</xdr:rowOff>
+      <xdr:rowOff>1330560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1082,8 +1126,452 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1586160" y="10353240"/>
-          <a:ext cx="484920" cy="1061640"/>
+          <a:off x="1408680" y="9999720"/>
+          <a:ext cx="1203840" cy="1669680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>32400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>408240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1251000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>960120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 2_0" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6343560" y="1414080"/>
+          <a:ext cx="1218600" cy="551880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2880</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>169920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1162800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 1_0" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1323000" y="1000440"/>
+          <a:ext cx="1579680" cy="1168200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1375200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>408240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>376560</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>960120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 2_2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14614200" y="1414080"/>
+          <a:ext cx="1218600" cy="551880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4680</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>169920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>455400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1162800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 1_2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9593640" y="1000440"/>
+          <a:ext cx="1579680" cy="1168200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1375200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>219240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>376560</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>771120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 2_4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14614200" y="7992000"/>
+          <a:ext cx="1218600" cy="551880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>117360</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>69480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>316080</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>1051200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Image 1_4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9706320" y="7842240"/>
+          <a:ext cx="1327680" cy="981720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>204120</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>746280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1232280</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1193400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 4_0" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId11"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6515280" y="4767480"/>
+          <a:ext cx="1028160" cy="447120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>150840</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>60120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>579600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1379520</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Image 3_0" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId12"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1470960" y="3731040"/>
+          <a:ext cx="1203840" cy="1669680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1547280</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>747720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>358200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1194840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Image 4_1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId13"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14786280" y="4768920"/>
+          <a:ext cx="1028160" cy="447120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152640</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>127080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>168120</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1364040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 3_1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId14"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9741600" y="3798000"/>
+          <a:ext cx="1144440" cy="1587240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1547280</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>750600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>358200</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1197720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Image 4_2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId15"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14786280" y="11089440"/>
+          <a:ext cx="1028160" cy="447120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>522000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>31320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>306000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1297440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Image 3_2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId16"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10110960" y="10370160"/>
+          <a:ext cx="912960" cy="1266120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1105,8 +1593,8 @@
   </sheetPr>
   <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A39" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E41" activeCellId="0" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1148,9 +1636,7 @@
       <c r="J2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1161,7 +1647,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1171,7 +1657,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -1181,7 +1667,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1191,7 +1677,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -1201,7 +1687,7 @@
     </row>
     <row r="6" customFormat="false" ht="98.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -1211,7 +1697,7 @@
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
       <c r="J6" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7"/>
@@ -1221,40 +1707,40 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="J7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="M7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="N7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="O7" s="9" t="s">
         <v>11</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,12 +1886,12 @@
       <c r="E13" s="11"/>
       <c r="F13" s="12"/>
       <c r="G13" s="9"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="16"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="11" t="n">
@@ -1420,48 +1906,48 @@
       <c r="E14" s="11"/>
       <c r="F14" s="12"/>
       <c r="G14" s="9"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="16"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="17"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="16"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="16"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="J16" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="18"/>
-      <c r="O16" s="18"/>
-    </row>
-    <row r="17" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="J16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+    </row>
+    <row r="17" customFormat="false" ht="108.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -1469,7 +1955,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="J17" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
@@ -1478,56 +1964,56 @@
       <c r="O17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="K18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="L18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="L18" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="M18" s="10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="N18" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O18" s="9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="13" t="n">
+      <c r="B19" s="11" t="n">
         <v>2.5</v>
       </c>
-      <c r="C19" s="14" t="n">
+      <c r="C19" s="11" t="n">
         <v>32.875</v>
       </c>
-      <c r="D19" s="14" t="n">
+      <c r="D19" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E19" s="14"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="16"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
       <c r="J19" s="11" t="n">
         <v>2</v>
       </c>
@@ -1542,18 +2028,18 @@
       <c r="O19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="13" t="n">
+      <c r="B20" s="11" t="n">
         <v>3.5</v>
       </c>
-      <c r="C20" s="14" t="n">
+      <c r="C20" s="11" t="n">
         <v>32.84375</v>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="16"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="9"/>
       <c r="J20" s="11" t="n">
         <v>4</v>
       </c>
@@ -1568,18 +2054,18 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="13" t="n">
+      <c r="B21" s="11" t="n">
         <v>4.5</v>
       </c>
-      <c r="C21" s="14" t="n">
+      <c r="C21" s="11" t="n">
         <v>32.78125</v>
       </c>
-      <c r="D21" s="14" t="n">
+      <c r="D21" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="16"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="9"/>
       <c r="J21" s="11" t="n">
         <v>6</v>
       </c>
@@ -1594,18 +2080,18 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="13" t="n">
+      <c r="B22" s="11" t="n">
         <v>5.5</v>
       </c>
-      <c r="C22" s="14" t="n">
+      <c r="C22" s="11" t="n">
         <v>32.75</v>
       </c>
-      <c r="D22" s="14" t="n">
+      <c r="D22" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="16"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="9"/>
       <c r="J22" s="11" t="n">
         <v>8</v>
       </c>
@@ -1620,18 +2106,18 @@
       <c r="O22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="13" t="n">
+      <c r="B23" s="11" t="n">
         <v>6.5</v>
       </c>
-      <c r="C23" s="14" t="n">
+      <c r="C23" s="11" t="n">
         <v>32.6875</v>
       </c>
-      <c r="D23" s="14" t="n">
+      <c r="D23" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="16"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="9"/>
       <c r="J23" s="11" t="n">
         <v>10</v>
       </c>
@@ -1646,146 +2132,146 @@
       <c r="O23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="13" t="n">
+      <c r="B24" s="11" t="n">
         <v>7.5</v>
       </c>
-      <c r="C24" s="14" t="n">
+      <c r="C24" s="11" t="n">
         <v>32.71875</v>
       </c>
-      <c r="D24" s="14" t="n">
+      <c r="D24" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="16"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="16"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="9"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="13" t="n">
+      <c r="B25" s="11" t="n">
         <v>8.5</v>
       </c>
-      <c r="C25" s="14" t="n">
+      <c r="C25" s="11" t="n">
         <v>32.625</v>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="11" t="n">
         <v>33</v>
       </c>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="16"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="16"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="9"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="15"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="21"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="23"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="23"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="21"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24"/>
+      <c r="A27" s="22"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24"/>
+      <c r="A28" s="22"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
-      <c r="J29" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
+      <c r="J29" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
-      <c r="J30" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
+      <c r="J30" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
     </row>
     <row r="31" customFormat="false" ht="89.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="J31" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="K31" s="27"/>
-      <c r="L31" s="27"/>
-      <c r="M31" s="27"/>
-      <c r="N31" s="27"/>
-      <c r="O31" s="27"/>
+      <c r="J31" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D32" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="F32" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="G32" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="K32" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="L32" s="30"/>
-      <c r="O32" s="31"/>
+      <c r="J32" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="K32" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L32" s="28"/>
+      <c r="O32" s="29"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="11" t="n">
@@ -1807,10 +2293,10 @@
         <v>0.255</v>
       </c>
       <c r="L33" s="11"/>
-      <c r="O33" s="31"/>
+      <c r="O33" s="29"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="32"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="11" t="n">
         <v>3.5</v>
       </c>
@@ -1830,7 +2316,7 @@
         <v>1.02</v>
       </c>
       <c r="L34" s="11"/>
-      <c r="O34" s="31"/>
+      <c r="O34" s="29"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="11" t="n">
@@ -1852,7 +2338,7 @@
         <v>1.755</v>
       </c>
       <c r="L35" s="11"/>
-      <c r="O35" s="31"/>
+      <c r="O35" s="29"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="11" t="n">
@@ -1874,7 +2360,7 @@
         <v>2.1</v>
       </c>
       <c r="L36" s="11"/>
-      <c r="O36" s="31"/>
+      <c r="O36" s="29"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="11" t="n">
@@ -1896,81 +2382,81 @@
         <v>2.53</v>
       </c>
       <c r="L37" s="11"/>
-      <c r="O37" s="31"/>
+      <c r="O37" s="29"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="13"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="16"/>
-      <c r="J38" s="33"/>
-      <c r="O38" s="31"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="15"/>
+      <c r="J38" s="31"/>
+      <c r="O38" s="29"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="J39" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
+      <c r="B39" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="16"/>
+      <c r="J39" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="24"/>
+      <c r="O39" s="24"/>
     </row>
     <row r="40" customFormat="false" ht="110.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B40" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-      <c r="J40" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="34"/>
-      <c r="N40" s="34"/>
-      <c r="O40" s="34"/>
+      <c r="J40" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="E41" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E41" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="F41" s="11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="K41" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="L41" s="37"/>
-      <c r="O41" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="J41" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="K41" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" s="35"/>
+      <c r="O41" s="29"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="11" t="n">
@@ -1992,7 +2478,7 @@
         <v>0.05</v>
       </c>
       <c r="L42" s="11"/>
-      <c r="O42" s="31"/>
+      <c r="O42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="11" t="n">
@@ -2014,7 +2500,7 @@
         <v>0.07</v>
       </c>
       <c r="L43" s="11"/>
-      <c r="O43" s="31"/>
+      <c r="O43" s="29"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="11" t="n">
@@ -2036,7 +2522,7 @@
         <v>0.08</v>
       </c>
       <c r="L44" s="11"/>
-      <c r="O44" s="31"/>
+      <c r="O44" s="29"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="11" t="n">
@@ -2058,7 +2544,7 @@
         <v>0.1</v>
       </c>
       <c r="L45" s="11"/>
-      <c r="O45" s="31"/>
+      <c r="O45" s="29"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="11" t="n">
@@ -2080,225 +2566,225 @@
         <v>0.12</v>
       </c>
       <c r="L46" s="11"/>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
-      <c r="O46" s="39"/>
+      <c r="M46" s="36"/>
+      <c r="N46" s="36"/>
+      <c r="O46" s="37"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="13"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="15"/>
-      <c r="G47" s="16"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="15"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="13"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="15"/>
-      <c r="G48" s="16"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="15"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="21"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
-      <c r="F49" s="22"/>
-      <c r="G49" s="23"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="21"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="40"/>
-      <c r="C55" s="40"/>
-      <c r="D55" s="40"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="40"/>
-      <c r="G55" s="40"/>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
     </row>
     <row r="56" customFormat="false" ht="81.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="41"/>
-      <c r="C56" s="41"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="41"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="39"/>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="15"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="15"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="14"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="15"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="14"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="15"/>
-      <c r="E67" s="15"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="40"/>
-      <c r="C68" s="40"/>
-      <c r="D68" s="40"/>
-      <c r="E68" s="40"/>
-      <c r="F68" s="40"/>
-      <c r="G68" s="40"/>
+      <c r="B68" s="38"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="38"/>
+      <c r="E68" s="38"/>
+      <c r="F68" s="38"/>
+      <c r="G68" s="38"/>
     </row>
     <row r="69" customFormat="false" ht="78" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B69" s="41"/>
-      <c r="C69" s="41"/>
-      <c r="D69" s="41"/>
-      <c r="E69" s="41"/>
-      <c r="F69" s="41"/>
-      <c r="G69" s="41"/>
+      <c r="B69" s="39"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="39"/>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="15"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="15"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="40"/>
+      <c r="D70" s="40"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="18"/>
+      <c r="G70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="15"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="41"/>
+      <c r="G71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="15"/>
-      <c r="G72" s="15"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="18"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="14"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-      <c r="F73" s="15"/>
-      <c r="G73" s="15"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-      <c r="F74" s="15"/>
-      <c r="G74" s="15"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="14"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="14"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-      <c r="F76" s="15"/>
-      <c r="G76" s="15"/>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="14"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-      <c r="F77" s="15"/>
-      <c r="G77" s="15"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="18"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="14"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="15"/>
-      <c r="C78" s="15"/>
-      <c r="D78" s="15"/>
-      <c r="E78" s="15"/>
-      <c r="F78" s="15"/>
-      <c r="G78" s="15"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="32">

</xml_diff>